<commit_message>
cotizacion casi lista, refactorizado backend y frontend
</commit_message>
<xml_diff>
--- a/server/assets/excel-imports/salonPacks_imp.xlsx
+++ b/server/assets/excel-imports/salonPacks_imp.xlsx
@@ -8,19 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ng388\Desktop\Audio Rental\audio-rental\server\assets\excel-imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA79CB9E-B8D9-49E5-ACFE-19D7529D87FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB7CE02-CA7C-4CEF-B3CD-41EC8A401255}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rubros" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="105">
   <si>
     <t>_id</t>
   </si>
@@ -34,12 +41,6 @@
     <t>mesanio</t>
   </si>
   <si>
-    <t>quincena1</t>
-  </si>
-  <si>
-    <t>quincena2</t>
-  </si>
-  <si>
     <t>5d4cfe9ec9a2f5adb832fe2a</t>
   </si>
   <si>
@@ -263,6 +264,84 @@
   </si>
   <si>
     <t>5d4cfe9ec9a2f5adb832fe6e</t>
+  </si>
+  <si>
+    <t>01-2019</t>
+  </si>
+  <si>
+    <t>02-2019</t>
+  </si>
+  <si>
+    <t>03-2019</t>
+  </si>
+  <si>
+    <t>04-2019</t>
+  </si>
+  <si>
+    <t>05-2019</t>
+  </si>
+  <si>
+    <t>06-2019</t>
+  </si>
+  <si>
+    <t>07-2019</t>
+  </si>
+  <si>
+    <t>08-2019</t>
+  </si>
+  <si>
+    <t>09-2019</t>
+  </si>
+  <si>
+    <t>10-2019</t>
+  </si>
+  <si>
+    <t>11-2019</t>
+  </si>
+  <si>
+    <t>12-2019</t>
+  </si>
+  <si>
+    <t>01-2020</t>
+  </si>
+  <si>
+    <t>02-2020</t>
+  </si>
+  <si>
+    <t>03-2020</t>
+  </si>
+  <si>
+    <t>04-2020</t>
+  </si>
+  <si>
+    <t>05-2020</t>
+  </si>
+  <si>
+    <t>06-2020</t>
+  </si>
+  <si>
+    <t>07-2020</t>
+  </si>
+  <si>
+    <t>08-2020</t>
+  </si>
+  <si>
+    <t>09-2020</t>
+  </si>
+  <si>
+    <t>10-2020</t>
+  </si>
+  <si>
+    <t>11-2020</t>
+  </si>
+  <si>
+    <t>12-2020</t>
+  </si>
+  <si>
+    <t>valorQuincena1</t>
+  </si>
+  <si>
+    <t>valorQuincena2</t>
   </si>
 </sst>
 </file>
@@ -643,9 +722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
@@ -653,7 +730,8 @@
     <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.92578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.35546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -670,24 +748,24 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1">
-        <v>43466</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E2">
         <v>85500</v>
@@ -698,16 +776,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1">
-        <v>43497</v>
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="E3">
         <v>85500</v>
@@ -718,16 +796,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1">
-        <v>43525</v>
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="E4">
         <v>85500</v>
@@ -738,16 +816,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1">
-        <v>43556</v>
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="E5">
         <v>85500</v>
@@ -758,16 +836,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1">
-        <v>43586</v>
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="E6">
         <v>85500</v>
@@ -778,16 +856,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="1">
-        <v>43617</v>
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E7">
         <v>85500</v>
@@ -798,16 +876,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="1">
-        <v>43647</v>
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="E8">
         <v>95500</v>
@@ -818,16 +896,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="1">
-        <v>43678</v>
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="E9">
         <v>95500</v>
@@ -838,16 +916,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="1">
-        <v>43709</v>
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="E10">
         <v>95500</v>
@@ -858,16 +936,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="1">
-        <v>43739</v>
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E11">
         <v>95500</v>
@@ -878,16 +956,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="1">
-        <v>43770</v>
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="E12">
         <v>95500</v>
@@ -898,16 +976,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="1">
-        <v>43800</v>
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="E13">
         <v>95500</v>
@@ -918,16 +996,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="1">
-        <v>43831</v>
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="E14">
         <v>98000</v>
@@ -938,16 +1016,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="1">
-        <v>43862</v>
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="E15">
         <v>101000</v>
@@ -958,16 +1036,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="1">
-        <v>43891</v>
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="E16">
         <v>107000</v>
@@ -978,16 +1056,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="1">
-        <v>43922</v>
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="E17">
         <v>110000</v>
@@ -998,16 +1076,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="1">
-        <v>43952</v>
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="E18">
         <v>112500</v>
@@ -1018,16 +1096,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="1">
-        <v>43983</v>
+        <v>6</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="E19">
         <v>115500</v>
@@ -1038,16 +1116,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="1">
-        <v>44013</v>
+        <v>6</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="E20">
         <v>118500</v>
@@ -1058,16 +1136,16 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="1">
-        <v>44044</v>
+        <v>6</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="E21">
         <v>121000</v>
@@ -1078,16 +1156,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="1">
-        <v>44075</v>
+        <v>6</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="E22">
         <v>124000</v>
@@ -1098,16 +1176,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="1">
-        <v>44105</v>
+        <v>6</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="E23">
         <v>127000</v>
@@ -1118,16 +1196,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="1">
-        <v>44136</v>
+        <v>6</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="E24">
         <v>130000</v>
@@ -1138,16 +1216,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="1">
-        <v>44166</v>
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="E25">
         <v>132000</v>
@@ -1158,16 +1236,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D26" s="1">
-        <v>43466</v>
+        <v>32</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E26">
         <v>85500</v>
@@ -1178,16 +1256,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="1">
-        <v>43497</v>
+        <v>32</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="E27">
         <v>85500</v>
@@ -1198,16 +1276,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="1">
-        <v>43525</v>
+        <v>32</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="E28">
         <v>85500</v>
@@ -1218,16 +1296,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="1">
-        <v>43556</v>
+        <v>32</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="E29">
         <v>85500</v>
@@ -1238,16 +1316,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" s="1">
-        <v>43586</v>
+        <v>32</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="E30">
         <v>85500</v>
@@ -1258,16 +1336,16 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
-      </c>
-      <c r="D31" s="1">
-        <v>43617</v>
+        <v>32</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E31">
         <v>85500</v>
@@ -1278,16 +1356,16 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32" s="1">
-        <v>43647</v>
+        <v>32</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="E32">
         <v>95500</v>
@@ -1298,16 +1376,16 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" s="1">
-        <v>43678</v>
+        <v>32</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="E33">
         <v>95500</v>
@@ -1318,16 +1396,16 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C34" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="1">
-        <v>43709</v>
+        <v>32</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="E34">
         <v>95500</v>
@@ -1338,16 +1416,16 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C35" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" s="1">
-        <v>43739</v>
+        <v>32</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E35">
         <v>95500</v>
@@ -1358,16 +1436,16 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
-      </c>
-      <c r="D36" s="1">
-        <v>43770</v>
+        <v>32</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="E36">
         <v>95500</v>
@@ -1378,16 +1456,16 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C37" t="s">
-        <v>34</v>
-      </c>
-      <c r="D37" s="1">
-        <v>43800</v>
+        <v>32</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="E37">
         <v>95500</v>
@@ -1398,16 +1476,16 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C38" t="s">
-        <v>34</v>
-      </c>
-      <c r="D38" s="1">
-        <v>43831</v>
+        <v>32</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="E38">
         <v>98000</v>
@@ -1418,16 +1496,16 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>34</v>
-      </c>
-      <c r="D39" s="1">
-        <v>43862</v>
+        <v>32</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="E39">
         <v>101000</v>
@@ -1438,16 +1516,16 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C40" t="s">
-        <v>34</v>
-      </c>
-      <c r="D40" s="1">
-        <v>43891</v>
+        <v>32</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="E40">
         <v>107000</v>
@@ -1458,16 +1536,16 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C41" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" s="1">
-        <v>43922</v>
+        <v>32</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="E41">
         <v>110000</v>
@@ -1478,16 +1556,16 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C42" t="s">
-        <v>34</v>
-      </c>
-      <c r="D42" s="1">
-        <v>43952</v>
+        <v>32</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="E42">
         <v>112500</v>
@@ -1498,16 +1576,16 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C43" t="s">
-        <v>34</v>
-      </c>
-      <c r="D43" s="1">
-        <v>43983</v>
+        <v>32</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="E43">
         <v>115500</v>
@@ -1518,16 +1596,16 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B44" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C44" t="s">
-        <v>34</v>
-      </c>
-      <c r="D44" s="1">
-        <v>44013</v>
+        <v>32</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="E44">
         <v>118500</v>
@@ -1538,16 +1616,16 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B45" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C45" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" s="1">
-        <v>44044</v>
+        <v>32</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="E45">
         <v>121000</v>
@@ -1558,16 +1636,16 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B46" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C46" t="s">
-        <v>34</v>
-      </c>
-      <c r="D46" s="1">
-        <v>44075</v>
+        <v>32</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="E46">
         <v>124000</v>
@@ -1578,16 +1656,16 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C47" t="s">
-        <v>34</v>
-      </c>
-      <c r="D47" s="1">
-        <v>44105</v>
+        <v>32</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="E47">
         <v>127000</v>
@@ -1598,16 +1676,16 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B48" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C48" t="s">
-        <v>34</v>
-      </c>
-      <c r="D48" s="1">
-        <v>44136</v>
+        <v>32</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>101</v>
       </c>
       <c r="E48">
         <v>130000</v>
@@ -1618,16 +1696,16 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C49" t="s">
-        <v>34</v>
-      </c>
-      <c r="D49" s="1">
-        <v>44166</v>
+        <v>32</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>102</v>
       </c>
       <c r="E49">
         <v>132000</v>
@@ -1638,16 +1716,16 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
+        <v>56</v>
+      </c>
+      <c r="B50" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50" t="s">
         <v>58</v>
       </c>
-      <c r="B50" t="s">
-        <v>59</v>
-      </c>
-      <c r="C50" t="s">
-        <v>60</v>
-      </c>
-      <c r="D50" s="1">
-        <v>43466</v>
+      <c r="D50" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="E50">
         <v>120750</v>
@@ -1658,16 +1736,16 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B51" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C51" t="s">
-        <v>60</v>
-      </c>
-      <c r="D51" s="1">
-        <v>43497</v>
+        <v>58</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="E51">
         <v>120750</v>
@@ -1678,16 +1756,16 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B52" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C52" t="s">
-        <v>60</v>
-      </c>
-      <c r="D52" s="1">
-        <v>43525</v>
+        <v>58</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="E52">
         <v>120750</v>
@@ -1698,16 +1776,16 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C53" t="s">
-        <v>60</v>
-      </c>
-      <c r="D53" s="1">
-        <v>43556</v>
+        <v>58</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="E53">
         <v>120750</v>
@@ -1718,16 +1796,16 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B54" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C54" t="s">
-        <v>60</v>
-      </c>
-      <c r="D54" s="1">
-        <v>43586</v>
+        <v>58</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="E54">
         <v>120750</v>
@@ -1738,16 +1816,16 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B55" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C55" t="s">
-        <v>60</v>
-      </c>
-      <c r="D55" s="1">
-        <v>43617</v>
+        <v>58</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="E55">
         <v>120750</v>
@@ -1758,16 +1836,16 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C56" t="s">
-        <v>60</v>
-      </c>
-      <c r="D56" s="1">
-        <v>43647</v>
+        <v>58</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="E56">
         <v>136500</v>
@@ -1778,16 +1856,16 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C57" t="s">
-        <v>60</v>
-      </c>
-      <c r="D57" s="1">
-        <v>43678</v>
+        <v>58</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="E57">
         <v>136500</v>
@@ -1798,16 +1876,16 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B58" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C58" t="s">
-        <v>60</v>
-      </c>
-      <c r="D58" s="1">
-        <v>43709</v>
+        <v>58</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="E58">
         <v>136500</v>
@@ -1818,16 +1896,16 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B59" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C59" t="s">
-        <v>60</v>
-      </c>
-      <c r="D59" s="1">
-        <v>43739</v>
+        <v>58</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E59">
         <v>136500</v>
@@ -1838,16 +1916,16 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B60" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C60" t="s">
-        <v>60</v>
-      </c>
-      <c r="D60" s="1">
-        <v>43770</v>
+        <v>58</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="E60">
         <v>136500</v>
@@ -1858,16 +1936,16 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B61" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C61" t="s">
-        <v>60</v>
-      </c>
-      <c r="D61" s="1">
-        <v>43800</v>
+        <v>58</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="E61">
         <v>136500</v>
@@ -1878,16 +1956,16 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C62" t="s">
-        <v>60</v>
-      </c>
-      <c r="D62" s="1">
-        <v>43831</v>
+        <v>58</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="E62">
         <v>140500</v>
@@ -1898,16 +1976,16 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B63" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C63" t="s">
-        <v>60</v>
-      </c>
-      <c r="D63" s="1">
-        <v>43862</v>
+        <v>58</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="E63">
         <v>145000</v>
@@ -1918,16 +1996,16 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B64" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C64" t="s">
-        <v>60</v>
-      </c>
-      <c r="D64" s="1">
-        <v>43891</v>
+        <v>58</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="E64">
         <v>153000</v>
@@ -1938,16 +2016,16 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B65" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C65" t="s">
-        <v>60</v>
-      </c>
-      <c r="D65" s="1">
-        <v>43922</v>
+        <v>58</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="E65">
         <v>157000</v>
@@ -1958,16 +2036,16 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B66" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C66" t="s">
-        <v>60</v>
-      </c>
-      <c r="D66" s="1">
-        <v>43952</v>
+        <v>58</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="E66">
         <v>161000</v>
@@ -1978,16 +2056,16 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B67" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C67" t="s">
-        <v>60</v>
-      </c>
-      <c r="D67" s="1">
-        <v>43983</v>
+        <v>58</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="E67">
         <v>165000</v>
@@ -1998,16 +2076,16 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B68" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C68" t="s">
-        <v>60</v>
-      </c>
-      <c r="D68" s="1">
-        <v>44013</v>
+        <v>58</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="E68">
         <v>169000</v>
@@ -2018,16 +2096,16 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B69" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C69" t="s">
-        <v>60</v>
-      </c>
-      <c r="D69" s="1">
-        <v>44044</v>
+        <v>58</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>98</v>
       </c>
       <c r="E69">
         <v>173000</v>
@@ -2038,16 +2116,16 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B70" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C70" t="s">
-        <v>60</v>
-      </c>
-      <c r="D70" s="1">
-        <v>44075</v>
+        <v>58</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="E70">
         <v>177500</v>
@@ -2058,8 +2136,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:F70" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:D1 A2:C70 E2:F70" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>